<commit_message>
elastic search : exemple requêtes
</commit_message>
<xml_diff>
--- a/1. StorageDatas/schemas.xlsx
+++ b/1. StorageDatas/schemas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="suivi" sheetId="9" r:id="rId1"/>
@@ -205,21 +205,6 @@
     <t>|-  copies : INTEGER</t>
   </si>
   <si>
-    <t>|-  sample_repo_name : STRING</t>
-  </si>
-  <si>
-    <t>|-  sample_ref : STRING</t>
-  </si>
-  <si>
-    <t>|-  sample_path : STRING</t>
-  </si>
-  <si>
-    <t>|-  sample_mode : INTEGER</t>
-  </si>
-  <si>
-    <t>|-  sample_symlink_target : STRING</t>
-  </si>
-  <si>
     <t>|-  ref : STRING</t>
   </si>
   <si>
@@ -308,9 +293,6 @@
   </si>
   <si>
     <t>Same as 'id' of 'files' table / Relation n --&gt; 1</t>
-  </si>
-  <si>
-    <t>Same as 'id' of 'contents' table / Relation 1 --&gt; n</t>
   </si>
   <si>
     <t>Leaf Field / Repeated</t>
@@ -364,9 +346,6 @@
   </si>
   <si>
     <t>Tables github demo : languages, licenses, repos_demo, githubarchive, commits, files, contents</t>
-  </si>
-  <si>
-    <t>|-  type : STRING</t>
   </si>
   <si>
     <t>|-  public : BOOLEAN</t>
@@ -512,6 +491,96 @@
   </si>
   <si>
     <t>SQL Field : language_bytes</t>
+  </si>
+  <si>
+    <t>Same as files.mode</t>
+  </si>
+  <si>
+    <t>Same as files.new_path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>CommitCommentEvent : commit_id &lt;-&gt; ['commits':commit]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Same as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>commits</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.difference.new_path</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Same as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>commits</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.diffrence.mode</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Same as 'id' of '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>contents</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' table / Relation 1 --&gt; n</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1270,7 +1339,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -1306,16 +1375,16 @@
     </row>
     <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E3" s="30"/>
       <c r="F3" s="30"/>
@@ -1331,16 +1400,16 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B4" s="12">
         <v>43155</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E4" s="33"/>
       <c r="F4" s="33"/>
@@ -1356,16 +1425,16 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B5" s="12">
         <v>43156</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E5" s="36"/>
       <c r="F5" s="36"/>
@@ -1381,16 +1450,16 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B6" s="12">
         <v>43162</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E6" s="23"/>
       <c r="F6" s="23"/>
@@ -1406,7 +1475,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="16"/>
@@ -1425,7 +1494,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="16"/>
@@ -1516,7 +1585,7 @@
   <dimension ref="B1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1529,13 +1598,13 @@
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="2:5" ht="77.25" x14ac:dyDescent="0.25">
@@ -1544,7 +1613,7 @@
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="21" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E2" s="1"/>
     </row>
@@ -1563,7 +1632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1576,13 +1645,13 @@
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
@@ -1592,7 +1661,7 @@
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>30</v>
@@ -1606,15 +1675,15 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C5" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1639,13 +1708,13 @@
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
@@ -1655,7 +1724,7 @@
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1667,8 +1736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:D22"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1676,18 +1745,18 @@
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1722,7 +1791,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1730,7 +1799,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1738,7 +1807,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1746,7 +1815,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1754,7 +1823,7 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1771,7 +1840,7 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1779,7 +1848,7 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1787,7 +1856,7 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1795,7 +1864,7 @@
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1803,7 +1872,7 @@
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1833,7 +1902,7 @@
         <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1841,7 +1910,7 @@
         <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1849,7 +1918,7 @@
         <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1869,7 +1938,7 @@
         <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1877,7 +1946,10 @@
         <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>64</v>
+        <v>59</v>
+      </c>
+      <c r="D25" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1885,7 +1957,7 @@
         <v>19</v>
       </c>
       <c r="C26" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1893,7 +1965,10 @@
         <v>20</v>
       </c>
       <c r="C27" t="s">
-        <v>66</v>
+        <v>61</v>
+      </c>
+      <c r="D27" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1901,7 +1976,7 @@
         <v>21</v>
       </c>
       <c r="C28" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1909,7 +1984,7 @@
         <v>22</v>
       </c>
       <c r="C29" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1917,7 +1992,7 @@
         <v>23</v>
       </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1925,7 +2000,7 @@
         <v>24</v>
       </c>
       <c r="C31" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1938,7 +2013,7 @@
         <v>26</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
@@ -1956,8 +2031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1969,13 +2044,13 @@
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
@@ -1985,17 +2060,23 @@
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
@@ -2003,12 +2084,12 @@
         <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>75</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -2018,10 +2099,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D11"/>
+  <dimension ref="B1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2033,13 +2114,13 @@
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
@@ -2047,7 +2128,7 @@
         <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
@@ -2068,31 +2149,6 @@
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -2104,46 +2160,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="32.5703125" customWidth="1"/>
     <col min="3" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>32</v>
@@ -2151,10 +2210,10 @@
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
@@ -2162,20 +2221,20 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C8" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>32</v>
@@ -2183,47 +2242,47 @@
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C10" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C11" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C12" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C13" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C14" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>32</v>
@@ -2231,47 +2290,47 @@
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C16" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C17" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C18" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C19" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" t="s">
         <v>110</v>
-      </c>
-      <c r="C20" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
@@ -2281,10 +2340,11 @@
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>